<commit_message>
AMC_multipar_comp separated from AMC_multipar_hw
Originariamente "AMC_multipar_hw" faceva il confronto tra tutti gli esempi in hardware
e tutti gli esempi in software. Ho rinominato questo file in "AMC_multipar_comp" e ho creato
un nuovo "AMC_multipar_hw" che e' identico ad "AMC_multipar" (quello in cui esegui l'AME su un singolo
esempio a scelta dell'utente) solo che ha le approssimazioni dell'architettura hardware (precisione finita).
</commit_message>
<xml_diff>
--- a/examples-tracking/matlab_examples-inventory.xlsx
+++ b/examples-tracking/matlab_examples-inventory.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>ExampleNum</t>
   </si>
@@ -140,6 +140,66 @@
   </si>
   <si>
     <t>Par</t>
+  </si>
+  <si>
+    <t>ExampleNum</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>.\sources\RaceHorses_416x240_30.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\VQ_sample_432x240.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\RaceHorses_416x240_30.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\VQ_sample_432x240.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\BasketballPass_416x240_50.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\VQ_sample_432x240.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\RaceHorses_416x240_30.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\BasketballPass_416x240_50.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\VQ_sample_432x240.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\BasketballPass_416x240_50.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\RaceHorses_416x240_30.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\BasketballPass_416x240_50.yuv</t>
+  </si>
+  <si>
+    <t>POC_Cur</t>
+  </si>
+  <si>
+    <t>x0</t>
+  </si>
+  <si>
+    <t>y0</t>
+  </si>
+  <si>
+    <t>Par</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -160,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -169,13 +229,15 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -490,7 +552,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="true" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
@@ -504,26 +566,34 @@
     <col min="4" max="4" width="4.140625" customWidth="true"/>
     <col min="6" max="6" width="4" customWidth="true"/>
     <col min="5" max="5" width="4.140625" customWidth="true"/>
+    <col min="7" max="7" width="3.140625" customWidth="true"/>
+    <col min="8" max="8" width="3.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2">
@@ -531,7 +601,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0">
         <v>4</v>
@@ -545,13 +615,19 @@
       <c r="F2" s="0">
         <v>4</v>
       </c>
+      <c r="G2" s="0">
+        <v>32</v>
+      </c>
+      <c r="H2" s="0">
+        <v>32</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C3" s="0">
         <v>4</v>
@@ -564,6 +640,12 @@
       </c>
       <c r="F3" s="0">
         <v>4</v>
+      </c>
+      <c r="G3" s="0">
+        <v>16</v>
+      </c>
+      <c r="H3" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -571,7 +653,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C4" s="0">
         <v>3</v>
@@ -584,6 +666,12 @@
       </c>
       <c r="F4" s="0">
         <v>4</v>
+      </c>
+      <c r="G4" s="0">
+        <v>32</v>
+      </c>
+      <c r="H4" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -591,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C5" s="0">
         <v>28</v>
@@ -604,6 +692,12 @@
       </c>
       <c r="F5" s="0">
         <v>4</v>
+      </c>
+      <c r="G5" s="0">
+        <v>16</v>
+      </c>
+      <c r="H5" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -611,7 +705,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0">
         <v>1</v>
@@ -624,6 +718,12 @@
       </c>
       <c r="F6" s="0">
         <v>6</v>
+      </c>
+      <c r="G6" s="0">
+        <v>32</v>
+      </c>
+      <c r="H6" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="7">
@@ -631,7 +731,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C7" s="0">
         <v>12</v>
@@ -644,6 +744,12 @@
       </c>
       <c r="F7" s="0">
         <v>6</v>
+      </c>
+      <c r="G7" s="0">
+        <v>32</v>
+      </c>
+      <c r="H7" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -651,7 +757,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0">
         <v>34</v>
@@ -664,6 +770,12 @@
       </c>
       <c r="F8" s="0">
         <v>6</v>
+      </c>
+      <c r="G8" s="0">
+        <v>32</v>
+      </c>
+      <c r="H8" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="9">
@@ -671,7 +783,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0">
         <v>49</v>
@@ -684,6 +796,12 @@
       </c>
       <c r="F9" s="0">
         <v>6</v>
+      </c>
+      <c r="G9" s="0">
+        <v>16</v>
+      </c>
+      <c r="H9" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -691,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C10" s="0">
         <v>1</v>
@@ -704,6 +822,12 @@
       </c>
       <c r="F10" s="0">
         <v>6</v>
+      </c>
+      <c r="G10" s="0">
+        <v>32</v>
+      </c>
+      <c r="H10" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="11">
@@ -711,7 +835,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0">
         <v>1</v>
@@ -724,6 +848,12 @@
       </c>
       <c r="F11" s="0">
         <v>6</v>
+      </c>
+      <c r="G11" s="0">
+        <v>32</v>
+      </c>
+      <c r="H11" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -731,7 +861,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C12" s="0">
         <v>1</v>
@@ -744,6 +874,12 @@
       </c>
       <c r="F12" s="0">
         <v>4</v>
+      </c>
+      <c r="G12" s="0">
+        <v>32</v>
+      </c>
+      <c r="H12" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="13">
@@ -751,7 +887,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C13" s="0">
         <v>1</v>
@@ -764,6 +900,12 @@
       </c>
       <c r="F13" s="0">
         <v>6</v>
+      </c>
+      <c r="G13" s="0">
+        <v>64</v>
+      </c>
+      <c r="H13" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="14">
@@ -771,7 +913,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C14" s="0">
         <v>2</v>
@@ -785,13 +927,19 @@
       <c r="F14" s="0">
         <v>4</v>
       </c>
+      <c r="G14" s="0">
+        <v>16</v>
+      </c>
+      <c r="H14" s="0">
+        <v>32</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
         <v>16</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C15" s="0">
         <v>1</v>
@@ -804,6 +952,12 @@
       </c>
       <c r="F15" s="0">
         <v>4</v>
+      </c>
+      <c r="G15" s="0">
+        <v>32</v>
+      </c>
+      <c r="H15" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="16">
@@ -811,7 +965,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C16" s="0">
         <v>1</v>
@@ -824,6 +978,12 @@
       </c>
       <c r="F16" s="0">
         <v>6</v>
+      </c>
+      <c r="G16" s="0">
+        <v>32</v>
+      </c>
+      <c r="H16" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="17">
@@ -831,7 +991,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C17" s="0">
         <v>2</v>
@@ -844,6 +1004,12 @@
       </c>
       <c r="F17" s="0">
         <v>4</v>
+      </c>
+      <c r="G17" s="0">
+        <v>32</v>
+      </c>
+      <c r="H17" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="18">
@@ -851,7 +1017,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C18" s="0">
         <v>2</v>
@@ -864,6 +1030,12 @@
       </c>
       <c r="F18" s="0">
         <v>4</v>
+      </c>
+      <c r="G18" s="0">
+        <v>32</v>
+      </c>
+      <c r="H18" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="19">
@@ -871,7 +1043,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C19" s="0">
         <v>5</v>
@@ -884,6 +1056,12 @@
       </c>
       <c r="F19" s="0">
         <v>4</v>
+      </c>
+      <c r="G19" s="0">
+        <v>64</v>
+      </c>
+      <c r="H19" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="20">
@@ -891,7 +1069,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C20" s="0">
         <v>7</v>
@@ -904,6 +1082,12 @@
       </c>
       <c r="F20" s="0">
         <v>6</v>
+      </c>
+      <c r="G20" s="0">
+        <v>16</v>
+      </c>
+      <c r="H20" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="21">
@@ -911,7 +1095,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C21" s="0">
         <v>3</v>
@@ -924,6 +1108,12 @@
       </c>
       <c r="F21" s="0">
         <v>6</v>
+      </c>
+      <c r="G21" s="0">
+        <v>32</v>
+      </c>
+      <c r="H21" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="22">
@@ -931,7 +1121,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C22" s="0">
         <v>4</v>
@@ -944,6 +1134,12 @@
       </c>
       <c r="F22" s="0">
         <v>6</v>
+      </c>
+      <c r="G22" s="0">
+        <v>32</v>
+      </c>
+      <c r="H22" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="23">
@@ -951,7 +1147,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C23" s="0">
         <v>4</v>
@@ -964,6 +1160,12 @@
       </c>
       <c r="F23" s="0">
         <v>4</v>
+      </c>
+      <c r="G23" s="0">
+        <v>32</v>
+      </c>
+      <c r="H23" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="24">
@@ -971,7 +1173,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C24" s="0">
         <v>25</v>
@@ -984,6 +1186,12 @@
       </c>
       <c r="F24" s="0">
         <v>6</v>
+      </c>
+      <c r="G24" s="0">
+        <v>16</v>
+      </c>
+      <c r="H24" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="25">
@@ -991,7 +1199,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C25" s="0">
         <v>29</v>
@@ -1004,6 +1212,12 @@
       </c>
       <c r="F25" s="0">
         <v>4</v>
+      </c>
+      <c r="G25" s="0">
+        <v>16</v>
+      </c>
+      <c r="H25" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="26">
@@ -1011,7 +1225,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C26" s="0">
         <v>3</v>
@@ -1024,6 +1238,12 @@
       </c>
       <c r="F26" s="0">
         <v>6</v>
+      </c>
+      <c r="G26" s="0">
+        <v>64</v>
+      </c>
+      <c r="H26" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="27">
@@ -1031,7 +1251,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C27" s="0">
         <v>5</v>
@@ -1044,6 +1264,12 @@
       </c>
       <c r="F27" s="0">
         <v>4</v>
+      </c>
+      <c r="G27" s="0">
+        <v>16</v>
+      </c>
+      <c r="H27" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="28">
@@ -1051,7 +1277,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C28" s="0">
         <v>38</v>
@@ -1064,6 +1290,12 @@
       </c>
       <c r="F28" s="0">
         <v>4</v>
+      </c>
+      <c r="G28" s="0">
+        <v>16</v>
+      </c>
+      <c r="H28" s="0">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DATA_MEMORY generator written succesfully
</commit_message>
<xml_diff>
--- a/examples-tracking/matlab_examples-inventory.xlsx
+++ b/examples-tracking/matlab_examples-inventory.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="78">
   <si>
     <t>ExampleNum</t>
   </si>
@@ -200,6 +200,72 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>ExampleNum</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>.\sources\RaceHorses_416x240_30.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\VQ_sample_432x240.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\RaceHorses_416x240_30.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\VQ_sample_432x240.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\BasketballPass_416x240_50.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\VQ_sample_432x240.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\RaceHorses_416x240_30.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\BasketballPass_416x240_50.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\VQ_sample_432x240.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\BasketballPass_416x240_50.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\RaceHorses_416x240_30.yuv</t>
+  </si>
+  <si>
+    <t>.\sources\BasketballPass_416x240_50.yuv</t>
+  </si>
+  <si>
+    <t>POC_Cur</t>
+  </si>
+  <si>
+    <t>x0</t>
+  </si>
+  <si>
+    <t>y0</t>
+  </si>
+  <si>
+    <t>Par</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>frame_w</t>
+  </si>
+  <si>
+    <t>frame_h</t>
   </si>
 </sst>
 </file>
@@ -220,7 +286,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -230,14 +296,16 @@
     </border>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -552,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="true" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
@@ -568,32 +636,40 @@
     <col min="5" max="5" width="4.140625" customWidth="true"/>
     <col min="7" max="7" width="3.140625" customWidth="true"/>
     <col min="8" max="8" width="3.140625" customWidth="true"/>
+    <col min="9" max="9" width="9" customWidth="true"/>
+    <col min="10" max="10" width="8.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>55</v>
+        <v>75</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2">
@@ -601,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0">
         <v>4</v>
@@ -621,13 +697,19 @@
       <c r="H2" s="0">
         <v>32</v>
       </c>
+      <c r="I2" s="0">
+        <v>416</v>
+      </c>
+      <c r="J2" s="0">
+        <v>240</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0">
         <v>4</v>
@@ -646,6 +728,12 @@
       </c>
       <c r="H3" s="0">
         <v>32</v>
+      </c>
+      <c r="I3" s="0">
+        <v>416</v>
+      </c>
+      <c r="J3" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="4">
@@ -653,7 +741,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C4" s="0">
         <v>3</v>
@@ -672,6 +760,12 @@
       </c>
       <c r="H4" s="0">
         <v>32</v>
+      </c>
+      <c r="I4" s="0">
+        <v>432</v>
+      </c>
+      <c r="J4" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="5">
@@ -679,7 +773,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C5" s="0">
         <v>28</v>
@@ -698,6 +792,12 @@
       </c>
       <c r="H5" s="0">
         <v>32</v>
+      </c>
+      <c r="I5" s="0">
+        <v>432</v>
+      </c>
+      <c r="J5" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="6">
@@ -705,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0">
         <v>1</v>
@@ -724,6 +824,12 @@
       </c>
       <c r="H6" s="0">
         <v>32</v>
+      </c>
+      <c r="I6" s="0">
+        <v>416</v>
+      </c>
+      <c r="J6" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="7">
@@ -731,7 +837,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C7" s="0">
         <v>12</v>
@@ -750,6 +856,12 @@
       </c>
       <c r="H7" s="0">
         <v>16</v>
+      </c>
+      <c r="I7" s="0">
+        <v>432</v>
+      </c>
+      <c r="J7" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="8">
@@ -757,7 +869,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C8" s="0">
         <v>34</v>
@@ -776,6 +888,12 @@
       </c>
       <c r="H8" s="0">
         <v>32</v>
+      </c>
+      <c r="I8" s="0">
+        <v>432</v>
+      </c>
+      <c r="J8" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="9">
@@ -783,7 +901,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C9" s="0">
         <v>49</v>
@@ -802,6 +920,12 @@
       </c>
       <c r="H9" s="0">
         <v>16</v>
+      </c>
+      <c r="I9" s="0">
+        <v>416</v>
+      </c>
+      <c r="J9" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="10">
@@ -809,7 +933,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C10" s="0">
         <v>1</v>
@@ -828,6 +952,12 @@
       </c>
       <c r="H10" s="0">
         <v>32</v>
+      </c>
+      <c r="I10" s="0">
+        <v>416</v>
+      </c>
+      <c r="J10" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="11">
@@ -835,7 +965,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C11" s="0">
         <v>1</v>
@@ -854,6 +984,12 @@
       </c>
       <c r="H11" s="0">
         <v>32</v>
+      </c>
+      <c r="I11" s="0">
+        <v>416</v>
+      </c>
+      <c r="J11" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="12">
@@ -861,7 +997,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C12" s="0">
         <v>1</v>
@@ -880,6 +1016,12 @@
       </c>
       <c r="H12" s="0">
         <v>32</v>
+      </c>
+      <c r="I12" s="0">
+        <v>416</v>
+      </c>
+      <c r="J12" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="13">
@@ -887,7 +1029,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C13" s="0">
         <v>1</v>
@@ -906,6 +1048,12 @@
       </c>
       <c r="H13" s="0">
         <v>32</v>
+      </c>
+      <c r="I13" s="0">
+        <v>432</v>
+      </c>
+      <c r="J13" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="14">
@@ -913,7 +1061,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C14" s="0">
         <v>2</v>
@@ -933,13 +1081,19 @@
       <c r="H14" s="0">
         <v>32</v>
       </c>
+      <c r="I14" s="0">
+        <v>432</v>
+      </c>
+      <c r="J14" s="0">
+        <v>240</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
         <v>16</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C15" s="0">
         <v>1</v>
@@ -958,6 +1112,12 @@
       </c>
       <c r="H15" s="0">
         <v>16</v>
+      </c>
+      <c r="I15" s="0">
+        <v>416</v>
+      </c>
+      <c r="J15" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="16">
@@ -965,7 +1125,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C16" s="0">
         <v>1</v>
@@ -984,6 +1144,12 @@
       </c>
       <c r="H16" s="0">
         <v>32</v>
+      </c>
+      <c r="I16" s="0">
+        <v>416</v>
+      </c>
+      <c r="J16" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="17">
@@ -991,7 +1157,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C17" s="0">
         <v>2</v>
@@ -1010,6 +1176,12 @@
       </c>
       <c r="H17" s="0">
         <v>32</v>
+      </c>
+      <c r="I17" s="0">
+        <v>416</v>
+      </c>
+      <c r="J17" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="18">
@@ -1017,7 +1189,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C18" s="0">
         <v>2</v>
@@ -1036,6 +1208,12 @@
       </c>
       <c r="H18" s="0">
         <v>16</v>
+      </c>
+      <c r="I18" s="0">
+        <v>416</v>
+      </c>
+      <c r="J18" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="19">
@@ -1043,7 +1221,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C19" s="0">
         <v>5</v>
@@ -1062,6 +1240,12 @@
       </c>
       <c r="H19" s="0">
         <v>16</v>
+      </c>
+      <c r="I19" s="0">
+        <v>416</v>
+      </c>
+      <c r="J19" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="20">
@@ -1069,7 +1253,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C20" s="0">
         <v>7</v>
@@ -1088,6 +1272,12 @@
       </c>
       <c r="H20" s="0">
         <v>32</v>
+      </c>
+      <c r="I20" s="0">
+        <v>416</v>
+      </c>
+      <c r="J20" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="21">
@@ -1095,7 +1285,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C21" s="0">
         <v>3</v>
@@ -1114,6 +1304,12 @@
       </c>
       <c r="H21" s="0">
         <v>32</v>
+      </c>
+      <c r="I21" s="0">
+        <v>432</v>
+      </c>
+      <c r="J21" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="22">
@@ -1121,7 +1317,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C22" s="0">
         <v>4</v>
@@ -1140,6 +1336,12 @@
       </c>
       <c r="H22" s="0">
         <v>16</v>
+      </c>
+      <c r="I22" s="0">
+        <v>432</v>
+      </c>
+      <c r="J22" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="23">
@@ -1147,7 +1349,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C23" s="0">
         <v>4</v>
@@ -1166,6 +1368,12 @@
       </c>
       <c r="H23" s="0">
         <v>16</v>
+      </c>
+      <c r="I23" s="0">
+        <v>432</v>
+      </c>
+      <c r="J23" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="24">
@@ -1173,7 +1381,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C24" s="0">
         <v>25</v>
@@ -1192,6 +1400,12 @@
       </c>
       <c r="H24" s="0">
         <v>32</v>
+      </c>
+      <c r="I24" s="0">
+        <v>416</v>
+      </c>
+      <c r="J24" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="25">
@@ -1199,7 +1413,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C25" s="0">
         <v>29</v>
@@ -1218,6 +1432,12 @@
       </c>
       <c r="H25" s="0">
         <v>16</v>
+      </c>
+      <c r="I25" s="0">
+        <v>416</v>
+      </c>
+      <c r="J25" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="26">
@@ -1225,7 +1445,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C26" s="0">
         <v>3</v>
@@ -1244,6 +1464,12 @@
       </c>
       <c r="H26" s="0">
         <v>32</v>
+      </c>
+      <c r="I26" s="0">
+        <v>416</v>
+      </c>
+      <c r="J26" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="27">
@@ -1251,7 +1477,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C27" s="0">
         <v>5</v>
@@ -1270,6 +1496,12 @@
       </c>
       <c r="H27" s="0">
         <v>16</v>
+      </c>
+      <c r="I27" s="0">
+        <v>416</v>
+      </c>
+      <c r="J27" s="0">
+        <v>240</v>
       </c>
     </row>
     <row r="28">
@@ -1277,7 +1509,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C28" s="0">
         <v>38</v>
@@ -1296,6 +1528,12 @@
       </c>
       <c r="H28" s="0">
         <v>16</v>
+      </c>
+      <c r="I28" s="0">
+        <v>416</v>
+      </c>
+      <c r="J28" s="0">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>